<commit_message>
price change for power bi
</commit_message>
<xml_diff>
--- a/All Scrapped Excels/Price id.xlsx
+++ b/All Scrapped Excels/Price id.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2.059,42 €</t>
+          <t xml:space="preserve">2.059,42 </t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -464,7 +464,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2.192,52 €</t>
+          <t xml:space="preserve">2.192,52 </t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.255,98 €</t>
+          <t xml:space="preserve">1.255,98 </t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -490,7 +490,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>568,70 €</t>
+          <t xml:space="preserve">568,70 </t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -503,7 +503,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.783,54 €</t>
+          <t xml:space="preserve">1.783,54 </t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -516,7 +516,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1.456,84 €</t>
+          <t xml:space="preserve">1.456,84 </t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -529,7 +529,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.456,84 €</t>
+          <t xml:space="preserve">1.456,84 </t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -542,7 +542,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1.588,73 €</t>
+          <t xml:space="preserve">1.588,73 </t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -555,7 +555,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1.032,13 €</t>
+          <t xml:space="preserve">1.032,13 </t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -568,7 +568,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1.553,64 €</t>
+          <t xml:space="preserve">1.553,64 </t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -581,7 +581,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1.779,91 €</t>
+          <t xml:space="preserve">1.779,91 </t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -594,7 +594,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1.206,37 €</t>
+          <t xml:space="preserve">1.206,37 </t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -607,7 +607,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>654,61 €</t>
+          <t xml:space="preserve">654,61 </t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -620,7 +620,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>711,48 €</t>
+          <t xml:space="preserve">711,48 </t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -633,7 +633,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1.783,54 €</t>
+          <t xml:space="preserve">1.783,54 </t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -646,7 +646,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>889,35 €</t>
+          <t xml:space="preserve">889,35 </t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -659,7 +659,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>670,34 €</t>
+          <t xml:space="preserve">670,34 </t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -672,7 +672,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>751,41 €</t>
+          <t xml:space="preserve">751,41 </t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -685,7 +685,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>790,13 €</t>
+          <t xml:space="preserve">790,13 </t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -698,7 +698,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>663,08 €</t>
+          <t xml:space="preserve">663,08 </t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -711,7 +711,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>497,31 €</t>
+          <t xml:space="preserve">497,31 </t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -724,7 +724,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1.472,57 €</t>
+          <t xml:space="preserve">1.472,57 </t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -737,7 +737,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1.386,66 €</t>
+          <t xml:space="preserve">1.386,66 </t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -750,7 +750,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>860,31 €</t>
+          <t xml:space="preserve">860,31 </t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1.073,27 €</t>
+          <t xml:space="preserve">1.073,27 </t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>699,38 €</t>
+          <t xml:space="preserve">699,38 </t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1.120,46 €</t>
+          <t xml:space="preserve">1.120,46 </t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -802,7 +802,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>821,59 €</t>
+          <t xml:space="preserve">821,59 </t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -815,7 +815,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>958,32 €</t>
+          <t xml:space="preserve">958,32 </t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -828,7 +828,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1.546,38 €</t>
+          <t xml:space="preserve">1.546,38 </t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1.724,25 €</t>
+          <t xml:space="preserve">1.724,25 </t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -854,7 +854,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2.004,97 €</t>
+          <t xml:space="preserve">2.004,97 </t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1.718,20 €</t>
+          <t xml:space="preserve">1.718,20 </t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1.362,46 €</t>
+          <t xml:space="preserve">1.362,46 </t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -893,7 +893,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1.361,25 €</t>
+          <t xml:space="preserve">1.361,25 </t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -906,7 +906,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>1.731,51 €</t>
+          <t xml:space="preserve">1.731,51 </t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1.886,39 €</t>
+          <t xml:space="preserve">1.886,39 </t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -932,7 +932,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2.088,46 €</t>
+          <t xml:space="preserve">2.088,46 </t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -945,7 +945,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>683,65 €</t>
+          <t xml:space="preserve">683,65 </t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -958,7 +958,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>707,85 €</t>
+          <t xml:space="preserve">707,85 </t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>705,43 €</t>
+          <t xml:space="preserve">705,43 </t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -984,7 +984,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>1.827,10 €</t>
+          <t xml:space="preserve">1.827,10 </t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -997,7 +997,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2.475,66 €</t>
+          <t xml:space="preserve">2.475,66 </t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>799,81 €</t>
+          <t xml:space="preserve">799,81 </t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2.105,40 €</t>
+          <t xml:space="preserve">2.105,40 </t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1.269,29 €</t>
+          <t xml:space="preserve">1.269,29 </t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>1.222,10 €</t>
+          <t xml:space="preserve">1.222,10 </t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>1.425,38 €</t>
+          <t xml:space="preserve">1.425,38 </t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>1.447,16 €</t>
+          <t xml:space="preserve">1.447,16 </t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>1.663,75 €</t>
+          <t xml:space="preserve">1.663,75 </t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>1.166,44 €</t>
+          <t xml:space="preserve">1.166,44 </t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>1.393,92 €</t>
+          <t xml:space="preserve">1.393,92 </t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1.070,85 €</t>
+          <t xml:space="preserve">1.070,85 </t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>1.318,90 €</t>
+          <t xml:space="preserve">1.318,90 </t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>1.295,91 €</t>
+          <t xml:space="preserve">1.295,91 </t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>778,03 €</t>
+          <t xml:space="preserve">778,03 </t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2.291,74 €</t>
+          <t xml:space="preserve">2.291,74 </t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>3.113,33 €</t>
+          <t xml:space="preserve">3.113,33 </t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>3.823,60 €</t>
+          <t xml:space="preserve">3.823,60 </t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>1.516,13 €</t>
+          <t xml:space="preserve">1.516,13 </t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>652,19 €</t>
+          <t xml:space="preserve">652,19 </t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>788,92 €</t>
+          <t xml:space="preserve">788,92 </t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>474,32 €</t>
+          <t xml:space="preserve">474,32 </t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>491,26 €</t>
+          <t xml:space="preserve">491,26 </t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>562,65 €</t>
+          <t xml:space="preserve">562,65 </t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>572,33 €</t>
+          <t xml:space="preserve">572,33 </t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>740,52 €</t>
+          <t xml:space="preserve">740,52 </t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1322,7 +1322,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>127,05 €</t>
+          <t xml:space="preserve">127,05 </t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>447,70 €</t>
+          <t xml:space="preserve">447,70 </t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>376,31 €</t>
+          <t xml:space="preserve">376,31 </t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>469,48 €</t>
+          <t xml:space="preserve">469,48 </t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>331,54 €</t>
+          <t xml:space="preserve">331,54 </t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1387,7 +1387,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>528,77 €</t>
+          <t xml:space="preserve">528,77 </t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>516,67 €</t>
+          <t xml:space="preserve">516,67 </t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1413,7 +1413,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>481,58 €</t>
+          <t xml:space="preserve">481,58 </t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1426,7 +1426,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>707,85 €</t>
+          <t xml:space="preserve">707,85 </t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>713,90 €</t>
+          <t xml:space="preserve">713,90 </t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>598,95 €</t>
+          <t xml:space="preserve">598,95 </t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>487,63 €</t>
+          <t xml:space="preserve">487,63 </t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>544,50 €</t>
+          <t xml:space="preserve">544,50 </t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>607,42 €</t>
+          <t xml:space="preserve">607,42 </t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1504,7 +1504,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>336,38 €</t>
+          <t xml:space="preserve">336,38 </t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>435,60 €</t>
+          <t xml:space="preserve">435,60 </t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1530,7 +1530,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>469,48 €</t>
+          <t xml:space="preserve">469,48 </t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>677,60 €</t>
+          <t xml:space="preserve">677,60 </t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>834,90 €</t>
+          <t xml:space="preserve">834,90 </t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>888,14 €</t>
+          <t xml:space="preserve">888,14 </t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1582,7 +1582,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>970,42 €</t>
+          <t xml:space="preserve">970,42 </t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1595,7 +1595,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>729,63 €</t>
+          <t xml:space="preserve">729,63 </t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>663,08 €</t>
+          <t xml:space="preserve">663,08 </t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>873,62 €</t>
+          <t xml:space="preserve">873,62 </t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1634,7 +1634,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>983,44 €</t>
+          <t xml:space="preserve">983,44 </t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1647,7 +1647,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>459,80 €</t>
+          <t xml:space="preserve">459,80 </t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>793,76 €</t>
+          <t xml:space="preserve">793,76 </t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>603,79 €</t>
+          <t xml:space="preserve">603,79 </t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -1686,7 +1686,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>647,35 €</t>
+          <t xml:space="preserve">647,35 </t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1699,7 +1699,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>926,86 €</t>
+          <t xml:space="preserve">926,86 </t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>496,10 €</t>
+          <t xml:space="preserve">496,10 </t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>565,07 €</t>
+          <t xml:space="preserve">565,07 </t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>615,89 €</t>
+          <t xml:space="preserve">615,89 </t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>733,26 €</t>
+          <t xml:space="preserve">733,26 </t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>959,53 €</t>
+          <t xml:space="preserve">959,53 </t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>742,94 €</t>
+          <t xml:space="preserve">742,94 </t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -1790,7 +1790,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>891,77 €</t>
+          <t xml:space="preserve">891,77 </t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>335,17 €</t>
+          <t xml:space="preserve">335,17 </t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>742,94 €</t>
+          <t xml:space="preserve">742,94 </t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>830,06 €</t>
+          <t xml:space="preserve">830,06 </t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>590,48 €</t>
+          <t xml:space="preserve">590,48 </t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>761,09 €</t>
+          <t xml:space="preserve">761,09 </t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>349,69 €</t>
+          <t xml:space="preserve">349,69 </t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>476,74 €</t>
+          <t xml:space="preserve">476,74 </t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -1894,7 +1894,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>338,80 €</t>
+          <t xml:space="preserve">338,80 </t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>430,76 €</t>
+          <t xml:space="preserve">430,76 </t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>235,95 €</t>
+          <t xml:space="preserve">235,95 </t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>474,32 €</t>
+          <t xml:space="preserve">474,32 </t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>485,21 €</t>
+          <t xml:space="preserve">485,21 </t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -1959,7 +1959,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>485,21 €</t>
+          <t xml:space="preserve">485,21 </t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>624,36 €</t>
+          <t xml:space="preserve">624,36 </t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>315,81 €</t>
+          <t xml:space="preserve">315,81 </t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -1998,7 +1998,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>350,90 €</t>
+          <t xml:space="preserve">350,90 </t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>330,33 €</t>
+          <t xml:space="preserve">330,33 </t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2024,7 +2024,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>392,04 €</t>
+          <t xml:space="preserve">392,04 </t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2037,7 +2037,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>206,91 €</t>
+          <t xml:space="preserve">206,91 </t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>434,39 €</t>
+          <t xml:space="preserve">434,39 </t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>326,70 €</t>
+          <t xml:space="preserve">326,70 </t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>473,11 €</t>
+          <t xml:space="preserve">473,11 </t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2089,7 +2089,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>988,57 €</t>
+          <t xml:space="preserve">988,57 </t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2102,7 +2102,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>751,41 €</t>
+          <t xml:space="preserve">751,41 </t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2115,7 +2115,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>629,20 €</t>
+          <t xml:space="preserve">629,20 </t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>758,67 €</t>
+          <t xml:space="preserve">758,67 </t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>652,19 €</t>
+          <t xml:space="preserve">652,19 </t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>784,08 €</t>
+          <t xml:space="preserve">784,08 </t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>988,57 €</t>
+          <t xml:space="preserve">988,57 </t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>717,53 €</t>
+          <t xml:space="preserve">717,53 </t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>1.022,45 €</t>
+          <t xml:space="preserve">1.022,45 </t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2206,7 +2206,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>820,38 €</t>
+          <t xml:space="preserve">820,38 </t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>880,88 €</t>
+          <t xml:space="preserve">880,88 </t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -2232,7 +2232,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>888,14 €</t>
+          <t xml:space="preserve">888,14 </t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2245,7 +2245,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>1.113,20 €</t>
+          <t xml:space="preserve">1.113,20 </t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>1.113,20 €</t>
+          <t xml:space="preserve">1.113,20 </t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>897,82 €</t>
+          <t xml:space="preserve">897,82 </t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>750,20 €</t>
+          <t xml:space="preserve">750,20 </t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -2297,7 +2297,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>1.274,13 €</t>
+          <t xml:space="preserve">1.274,13 </t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2310,7 +2310,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>1.195,48 €</t>
+          <t xml:space="preserve">1.195,48 </t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>1.172,49 €</t>
+          <t xml:space="preserve">1.172,49 </t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>1.174,91 €</t>
+          <t xml:space="preserve">1.174,91 </t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -2349,7 +2349,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>1.286,23 €</t>
+          <t xml:space="preserve">1.286,23 </t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -2362,7 +2362,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>1.255,98 €</t>
+          <t xml:space="preserve">1.255,98 </t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2375,7 +2375,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>1.219,68 €</t>
+          <t xml:space="preserve">1.219,68 </t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2388,7 +2388,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>1.247,51 €</t>
+          <t xml:space="preserve">1.247,51 </t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>1.201,53 €</t>
+          <t xml:space="preserve">1.201,53 </t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2414,7 +2414,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>482,79 €</t>
+          <t xml:space="preserve">482,79 </t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>456,17 €</t>
+          <t xml:space="preserve">456,17 </t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>646,14 €</t>
+          <t xml:space="preserve">646,14 </t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>658,24 €</t>
+          <t xml:space="preserve">658,24 </t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2466,7 +2466,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>671,55 €</t>
+          <t xml:space="preserve">671,55 </t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2479,7 +2479,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>762,30 €</t>
+          <t xml:space="preserve">762,30 </t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2492,7 +2492,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>834,90 €</t>
+          <t xml:space="preserve">834,90 </t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>447,70 €</t>
+          <t xml:space="preserve">447,70 </t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>905,08 €</t>
+          <t xml:space="preserve">905,08 </t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2531,7 +2531,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>889,35 €</t>
+          <t xml:space="preserve">889,35 </t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -2544,7 +2544,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>976,47 €</t>
+          <t xml:space="preserve">976,47 </t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>640,09 €</t>
+          <t xml:space="preserve">640,09 </t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -2570,7 +2570,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>713,90 €</t>
+          <t xml:space="preserve">713,90 </t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>746,57 €</t>
+          <t xml:space="preserve">746,57 </t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>592,90 €</t>
+          <t xml:space="preserve">592,90 </t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2609,7 +2609,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>572,33 €</t>
+          <t xml:space="preserve">572,33 </t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -2622,7 +2622,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>652,19 €</t>
+          <t xml:space="preserve">652,19 </t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>802,23 €</t>
+          <t xml:space="preserve">802,23 </t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -2648,7 +2648,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>865,14 €</t>
+          <t xml:space="preserve">865,14 </t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>671,55 €</t>
+          <t xml:space="preserve">671,55 </t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -2674,7 +2674,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>592,90 €</t>
+          <t xml:space="preserve">592,90 </t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>1.621,40 €</t>
+          <t xml:space="preserve">1.621,40 </t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -2700,7 +2700,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>943,80 €</t>
+          <t xml:space="preserve">943,80 </t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>815,54 €</t>
+          <t xml:space="preserve">815,54 </t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>895,40 €</t>
+          <t xml:space="preserve">895,40 </t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>1.040,60 €</t>
+          <t xml:space="preserve">1.040,60 </t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -2752,7 +2752,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>1.379,40 €</t>
+          <t xml:space="preserve">1.379,40 </t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>1.229,36 €</t>
+          <t xml:space="preserve">1.229,36 </t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -2778,7 +2778,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>863,94 €</t>
+          <t xml:space="preserve">863,94 </t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>513,04 €</t>
+          <t xml:space="preserve">513,04 </t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>496,10 €</t>
+          <t xml:space="preserve">496,10 </t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>549,34 €</t>
+          <t xml:space="preserve">549,34 </t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>629,20 €</t>
+          <t xml:space="preserve">629,20 </t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>331,54 €</t>
+          <t xml:space="preserve">331,54 </t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -2856,7 +2856,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>900,24 €</t>
+          <t xml:space="preserve">900,24 </t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -2869,7 +2869,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>425,92 €</t>
+          <t xml:space="preserve">425,92 </t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>358,16 €</t>
+          <t xml:space="preserve">358,16 </t>
         </is>
       </c>
       <c r="C189" t="n">
@@ -2895,7 +2895,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>304,92 €</t>
+          <t xml:space="preserve">304,92 </t>
         </is>
       </c>
       <c r="C190" t="n">
@@ -2908,7 +2908,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>484,00 €</t>
+          <t xml:space="preserve">484,00 </t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -2921,7 +2921,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>592,90 €</t>
+          <t xml:space="preserve">592,90 </t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -2934,7 +2934,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>590,48 €</t>
+          <t xml:space="preserve">590,48 </t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>706,64 €</t>
+          <t xml:space="preserve">706,64 </t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -2960,7 +2960,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>515,46 €</t>
+          <t xml:space="preserve">515,46 </t>
         </is>
       </c>
       <c r="C195" t="n">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>629,20 €</t>
+          <t xml:space="preserve">629,20 </t>
         </is>
       </c>
       <c r="C196" t="n">
@@ -2986,7 +2986,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>793,76 €</t>
+          <t xml:space="preserve">793,76 </t>
         </is>
       </c>
       <c r="C197" t="n">
@@ -2999,7 +2999,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>447,70 €</t>
+          <t xml:space="preserve">447,70 </t>
         </is>
       </c>
       <c r="C198" t="n">
@@ -3012,7 +3012,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>423,50 €</t>
+          <t xml:space="preserve">423,50 </t>
         </is>
       </c>
       <c r="C199" t="n">
@@ -3025,7 +3025,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>392,04 €</t>
+          <t xml:space="preserve">392,04 </t>
         </is>
       </c>
       <c r="C200" t="n">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>338,80 €</t>
+          <t xml:space="preserve">338,80 </t>
         </is>
       </c>
       <c r="C201" t="n">
@@ -3051,7 +3051,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>459,80 €</t>
+          <t xml:space="preserve">459,80 </t>
         </is>
       </c>
       <c r="C202" t="n">
@@ -3064,7 +3064,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>350,90 €</t>
+          <t xml:space="preserve">350,90 </t>
         </is>
       </c>
       <c r="C203" t="n">
@@ -3077,7 +3077,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>851,84 €</t>
+          <t xml:space="preserve">851,84 </t>
         </is>
       </c>
       <c r="C204" t="n">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>605,00 €</t>
+          <t xml:space="preserve">605,00 </t>
         </is>
       </c>
       <c r="C205" t="n">
@@ -3103,7 +3103,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>561,44 €</t>
+          <t xml:space="preserve">561,44 </t>
         </is>
       </c>
       <c r="C206" t="n">
@@ -3116,7 +3116,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>508,20 €</t>
+          <t xml:space="preserve">508,20 </t>
         </is>
       </c>
       <c r="C207" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>568,70 €</t>
+          <t xml:space="preserve">568,70 </t>
         </is>
       </c>
       <c r="C208" t="n">
@@ -3142,7 +3142,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>416,24 €</t>
+          <t xml:space="preserve">416,24 </t>
         </is>
       </c>
       <c r="C209" t="n">
@@ -3155,7 +3155,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>219,01 €</t>
+          <t xml:space="preserve">219,01 </t>
         </is>
       </c>
       <c r="C210" t="n">
@@ -3168,7 +3168,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>249,26 €</t>
+          <t xml:space="preserve">249,26 </t>
         </is>
       </c>
       <c r="C211" t="n">
@@ -3181,7 +3181,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>329,12 €</t>
+          <t xml:space="preserve">329,12 </t>
         </is>
       </c>
       <c r="C212" t="n">
@@ -3194,7 +3194,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>193,60 €</t>
+          <t xml:space="preserve">193,60 </t>
         </is>
       </c>
       <c r="C213" t="n">
@@ -3207,7 +3207,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>186,34 €</t>
+          <t xml:space="preserve">186,34 </t>
         </is>
       </c>
       <c r="C214" t="n">
@@ -3220,7 +3220,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>422,29 €</t>
+          <t xml:space="preserve">422,29 </t>
         </is>
       </c>
       <c r="C215" t="n">
@@ -3233,7 +3233,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>355,74 €</t>
+          <t xml:space="preserve">355,74 </t>
         </is>
       </c>
       <c r="C216" t="n">
@@ -3246,7 +3246,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>329,12 €</t>
+          <t xml:space="preserve">329,12 </t>
         </is>
       </c>
       <c r="C217" t="n">
@@ -3259,7 +3259,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>249,26 €</t>
+          <t xml:space="preserve">249,26 </t>
         </is>
       </c>
       <c r="C218" t="n">
@@ -3272,7 +3272,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>384,78 €</t>
+          <t xml:space="preserve">384,78 </t>
         </is>
       </c>
       <c r="C219" t="n">
@@ -3285,7 +3285,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>187,55 €</t>
+          <t xml:space="preserve">187,55 </t>
         </is>
       </c>
       <c r="C220" t="n">
@@ -3298,7 +3298,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>237,16 €</t>
+          <t xml:space="preserve">237,16 </t>
         </is>
       </c>
       <c r="C221" t="n">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>655,82 €</t>
+          <t xml:space="preserve">655,82 </t>
         </is>
       </c>
       <c r="C222" t="n">
@@ -3324,7 +3324,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>769,56 €</t>
+          <t xml:space="preserve">769,56 </t>
         </is>
       </c>
       <c r="C223" t="n">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>677,60 €</t>
+          <t xml:space="preserve">677,60 </t>
         </is>
       </c>
       <c r="C224" t="n">
@@ -3350,7 +3350,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>597,74 €</t>
+          <t xml:space="preserve">597,74 </t>
         </is>
       </c>
       <c r="C225" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>688,49 €</t>
+          <t xml:space="preserve">688,49 </t>
         </is>
       </c>
       <c r="C226" t="n">
@@ -3376,7 +3376,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>837,32 €</t>
+          <t xml:space="preserve">837,32 </t>
         </is>
       </c>
       <c r="C227" t="n">
@@ -3389,7 +3389,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>242,00 €</t>
+          <t xml:space="preserve">242,00 </t>
         </is>
       </c>
       <c r="C228" t="n">
@@ -3402,7 +3402,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>291,61 €</t>
+          <t xml:space="preserve">291,61 </t>
         </is>
       </c>
       <c r="C229" t="n">
@@ -3415,7 +3415,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>407,77 €</t>
+          <t xml:space="preserve">407,77 </t>
         </is>
       </c>
       <c r="C230" t="n">
@@ -3428,7 +3428,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>479,16 €</t>
+          <t xml:space="preserve">479,16 </t>
         </is>
       </c>
       <c r="C231" t="n">
@@ -3441,7 +3441,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>152,46 €</t>
+          <t xml:space="preserve">152,46 </t>
         </is>
       </c>
       <c r="C232" t="n">
@@ -3454,7 +3454,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>327,91 €</t>
+          <t xml:space="preserve">327,91 </t>
         </is>
       </c>
       <c r="C233" t="n">
@@ -3467,7 +3467,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>326,70 €</t>
+          <t xml:space="preserve">326,70 </t>
         </is>
       </c>
       <c r="C234" t="n">
@@ -3480,7 +3480,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>304,92 €</t>
+          <t xml:space="preserve">304,92 </t>
         </is>
       </c>
       <c r="C235" t="n">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>220,22 €</t>
+          <t xml:space="preserve">220,22 </t>
         </is>
       </c>
       <c r="C236" t="n">
@@ -3506,7 +3506,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>395,67 €</t>
+          <t xml:space="preserve">395,67 </t>
         </is>
       </c>
       <c r="C237" t="n">
@@ -3519,7 +3519,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>394,46 €</t>
+          <t xml:space="preserve">394,46 </t>
         </is>
       </c>
       <c r="C238" t="n">
@@ -3532,7 +3532,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>388,41 €</t>
+          <t xml:space="preserve">388,41 </t>
         </is>
       </c>
       <c r="C239" t="n">
@@ -3545,7 +3545,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>586,85 €</t>
+          <t xml:space="preserve">586,85 </t>
         </is>
       </c>
       <c r="C240" t="n">
@@ -3558,7 +3558,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>572,33 €</t>
+          <t xml:space="preserve">572,33 </t>
         </is>
       </c>
       <c r="C241" t="n">
@@ -3571,7 +3571,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>424,71 €</t>
+          <t xml:space="preserve">424,71 </t>
         </is>
       </c>
       <c r="C242" t="n">
@@ -3584,7 +3584,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>486,42 €</t>
+          <t xml:space="preserve">486,42 </t>
         </is>
       </c>
       <c r="C243" t="n">
@@ -3597,7 +3597,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>765,93 €</t>
+          <t xml:space="preserve">765,93 </t>
         </is>
       </c>
       <c r="C244" t="n">
@@ -3610,7 +3610,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>931,70 €</t>
+          <t xml:space="preserve">931,70 </t>
         </is>
       </c>
       <c r="C245" t="n">
@@ -3623,7 +3623,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>774,40 €</t>
+          <t xml:space="preserve">774,40 </t>
         </is>
       </c>
       <c r="C246" t="n">
@@ -3636,7 +3636,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>681,23 €</t>
+          <t xml:space="preserve">681,23 </t>
         </is>
       </c>
       <c r="C247" t="n">
@@ -3649,7 +3649,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>845,79 €</t>
+          <t xml:space="preserve">845,79 </t>
         </is>
       </c>
       <c r="C248" t="n">
@@ -3662,7 +3662,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>688,49 €</t>
+          <t xml:space="preserve">688,49 </t>
         </is>
       </c>
       <c r="C249" t="n">
@@ -3675,7 +3675,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>629,20 €</t>
+          <t xml:space="preserve">629,20 </t>
         </is>
       </c>
       <c r="C250" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>794,97 €</t>
+          <t xml:space="preserve">794,97 </t>
         </is>
       </c>
       <c r="C251" t="n">
@@ -3701,7 +3701,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>637,67 €</t>
+          <t xml:space="preserve">637,67 </t>
         </is>
       </c>
       <c r="C252" t="n">
@@ -3714,7 +3714,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>606,21 €</t>
+          <t xml:space="preserve">606,21 </t>
         </is>
       </c>
       <c r="C253" t="n">
@@ -3727,7 +3727,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>732,05 €</t>
+          <t xml:space="preserve">732,05 </t>
         </is>
       </c>
       <c r="C254" t="n">
@@ -3740,7 +3740,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>704,22 €</t>
+          <t xml:space="preserve">704,22 </t>
         </is>
       </c>
       <c r="C255" t="n">
@@ -3753,7 +3753,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>773,19 €</t>
+          <t xml:space="preserve">773,19 </t>
         </is>
       </c>
       <c r="C256" t="n">
@@ -3766,7 +3766,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>615,89 €</t>
+          <t xml:space="preserve">615,89 </t>
         </is>
       </c>
       <c r="C257" t="n">
@@ -3779,7 +3779,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>607,42 €</t>
+          <t xml:space="preserve">607,42 </t>
         </is>
       </c>
       <c r="C258" t="n">
@@ -3792,7 +3792,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>504,57 €</t>
+          <t xml:space="preserve">504,57 </t>
         </is>
       </c>
       <c r="C259" t="n">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>555,39 €</t>
+          <t xml:space="preserve">555,39 </t>
         </is>
       </c>
       <c r="C260" t="n">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>648,56 €</t>
+          <t xml:space="preserve">648,56 </t>
         </is>
       </c>
       <c r="C261" t="n">
@@ -3831,7 +3831,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>687,28 €</t>
+          <t xml:space="preserve">687,28 </t>
         </is>
       </c>
       <c r="C262" t="n">
@@ -3844,7 +3844,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>758,67 €</t>
+          <t xml:space="preserve">758,67 </t>
         </is>
       </c>
       <c r="C263" t="n">
@@ -3857,7 +3857,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>778,03 €</t>
+          <t xml:space="preserve">778,03 </t>
         </is>
       </c>
       <c r="C264" t="n">
@@ -3870,7 +3870,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>808,28 €</t>
+          <t xml:space="preserve">808,28 </t>
         </is>
       </c>
       <c r="C265" t="n">
@@ -3883,7 +3883,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>635,25 €</t>
+          <t xml:space="preserve">635,25 </t>
         </is>
       </c>
       <c r="C266" t="n">
@@ -3896,7 +3896,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>694,54 €</t>
+          <t xml:space="preserve">694,54 </t>
         </is>
       </c>
       <c r="C267" t="n">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>716,32 €</t>
+          <t xml:space="preserve">716,32 </t>
         </is>
       </c>
       <c r="C268" t="n">
@@ -3922,7 +3922,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>807,07 €</t>
+          <t xml:space="preserve">807,07 </t>
         </is>
       </c>
       <c r="C269" t="n">
@@ -3935,7 +3935,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>222,64 €</t>
+          <t xml:space="preserve">222,64 </t>
         </is>
       </c>
       <c r="C270" t="n">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>726,00 €</t>
+          <t xml:space="preserve">726,00 </t>
         </is>
       </c>
       <c r="C271" t="n">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>212,96 €</t>
+          <t xml:space="preserve">212,96 </t>
         </is>
       </c>
       <c r="C272" t="n">
@@ -3974,7 +3974,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>453,75 €</t>
+          <t xml:space="preserve">453,75 </t>
         </is>
       </c>
       <c r="C273" t="n">
@@ -3987,7 +3987,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>482,79 €</t>
+          <t xml:space="preserve">482,79 </t>
         </is>
       </c>
       <c r="C274" t="n">
@@ -4000,7 +4000,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>278,30 €</t>
+          <t xml:space="preserve">278,30 </t>
         </is>
       </c>
       <c r="C275" t="n">
@@ -4013,7 +4013,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>402,93 €</t>
+          <t xml:space="preserve">402,93 </t>
         </is>
       </c>
       <c r="C276" t="n">
@@ -4026,7 +4026,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>643,72 €</t>
+          <t xml:space="preserve">643,72 </t>
         </is>
       </c>
       <c r="C277" t="n">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>672,76 €</t>
+          <t xml:space="preserve">672,76 </t>
         </is>
       </c>
       <c r="C278" t="n">
@@ -4052,7 +4052,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>355,74 €</t>
+          <t xml:space="preserve">355,74 </t>
         </is>
       </c>
       <c r="C279" t="n">
@@ -4065,7 +4065,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>519,09 €</t>
+          <t xml:space="preserve">519,09 </t>
         </is>
       </c>
       <c r="C280" t="n">
@@ -4078,7 +4078,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>596,53 €</t>
+          <t xml:space="preserve">596,53 </t>
         </is>
       </c>
       <c r="C281" t="n">
@@ -4091,7 +4091,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>625,57 €</t>
+          <t xml:space="preserve">625,57 </t>
         </is>
       </c>
       <c r="C282" t="n">
@@ -4104,7 +4104,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>548,13 €</t>
+          <t xml:space="preserve">548,13 </t>
         </is>
       </c>
       <c r="C283" t="n">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>523,93 €</t>
+          <t xml:space="preserve">523,93 </t>
         </is>
       </c>
       <c r="C284" t="n">
@@ -4130,7 +4130,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>792,55 €</t>
+          <t xml:space="preserve">792,55 </t>
         </is>
       </c>
       <c r="C285" t="n">
@@ -4143,7 +4143,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>764,72 €</t>
+          <t xml:space="preserve">764,72 </t>
         </is>
       </c>
       <c r="C286" t="n">
@@ -4156,7 +4156,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>263,78 €</t>
+          <t xml:space="preserve">263,78 </t>
         </is>
       </c>
       <c r="C287" t="n">
@@ -4169,7 +4169,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>592,90 €</t>
+          <t xml:space="preserve">592,90 </t>
         </is>
       </c>
       <c r="C288" t="n">
@@ -4182,7 +4182,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>292,82 €</t>
+          <t xml:space="preserve">292,82 </t>
         </is>
       </c>
       <c r="C289" t="n">
@@ -4195,7 +4195,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>1.074,48 €</t>
+          <t xml:space="preserve">1.074,48 </t>
         </is>
       </c>
       <c r="C290" t="n">
@@ -4208,7 +4208,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>353,32 €</t>
+          <t xml:space="preserve">353,32 </t>
         </is>
       </c>
       <c r="C291" t="n">
@@ -4221,7 +4221,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>739,31 €</t>
+          <t xml:space="preserve">739,31 </t>
         </is>
       </c>
       <c r="C292" t="n">
@@ -4234,7 +4234,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>965,58 €</t>
+          <t xml:space="preserve">965,58 </t>
         </is>
       </c>
       <c r="C293" t="n">
@@ -4247,7 +4247,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>908,71 €</t>
+          <t xml:space="preserve">908,71 </t>
         </is>
       </c>
       <c r="C294" t="n">
@@ -4260,7 +4260,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>621,94 €</t>
+          <t xml:space="preserve">621,94 </t>
         </is>
       </c>
       <c r="C295" t="n">
@@ -4273,7 +4273,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>475,53 €</t>
+          <t xml:space="preserve">475,53 </t>
         </is>
       </c>
       <c r="C296" t="n">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>886,93 €</t>
+          <t xml:space="preserve">886,93 </t>
         </is>
       </c>
       <c r="C297" t="n">
@@ -4299,7 +4299,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>445,28 €</t>
+          <t xml:space="preserve">445,28 </t>
         </is>
       </c>
       <c r="C298" t="n">
@@ -4312,7 +4312,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>669,13 €</t>
+          <t xml:space="preserve">669,13 </t>
         </is>
       </c>
       <c r="C299" t="n">
@@ -4325,7 +4325,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>1.056,33 €</t>
+          <t xml:space="preserve">1.056,33 </t>
         </is>
       </c>
       <c r="C300" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>1.057,54 €</t>
+          <t xml:space="preserve">1.057,54 </t>
         </is>
       </c>
       <c r="C301" t="n">
@@ -4351,7 +4351,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>204,49 €</t>
+          <t xml:space="preserve">204,49 </t>
         </is>
       </c>
       <c r="C302" t="n">
@@ -4364,7 +4364,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>1.216,05 €</t>
+          <t xml:space="preserve">1.216,05 </t>
         </is>
       </c>
       <c r="C303" t="n">
@@ -4377,7 +4377,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>474,32 €</t>
+          <t xml:space="preserve">474,32 </t>
         </is>
       </c>
       <c r="C304" t="n">
@@ -4390,7 +4390,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>203,28 €</t>
+          <t xml:space="preserve">203,28 </t>
         </is>
       </c>
       <c r="C305" t="n">
@@ -4403,7 +4403,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>1.155,55 €</t>
+          <t xml:space="preserve">1.155,55 </t>
         </is>
       </c>
       <c r="C306" t="n">
@@ -4416,7 +4416,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>271,04 €</t>
+          <t xml:space="preserve">271,04 </t>
         </is>
       </c>
       <c r="C307" t="n">
@@ -4429,7 +4429,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>2.250,60 €</t>
+          <t xml:space="preserve">2.250,60 </t>
         </is>
       </c>
       <c r="C308" t="n">
@@ -4442,7 +4442,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>3.037,10 €</t>
+          <t xml:space="preserve">3.037,10 </t>
         </is>
       </c>
       <c r="C309" t="n">
@@ -4455,7 +4455,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>325,49 €</t>
+          <t xml:space="preserve">325,49 </t>
         </is>
       </c>
       <c r="C310" t="n">
@@ -4468,7 +4468,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>206,91 €</t>
+          <t xml:space="preserve">206,91 </t>
         </is>
       </c>
       <c r="C311" t="n">
@@ -4481,7 +4481,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>297,66 €</t>
+          <t xml:space="preserve">297,66 </t>
         </is>
       </c>
       <c r="C312" t="n">
@@ -4494,7 +4494,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>306,13 €</t>
+          <t xml:space="preserve">306,13 </t>
         </is>
       </c>
       <c r="C313" t="n">
@@ -4507,7 +4507,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>394,46 €</t>
+          <t xml:space="preserve">394,46 </t>
         </is>
       </c>
       <c r="C314" t="n">
@@ -4520,7 +4520,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>526,35 €</t>
+          <t xml:space="preserve">526,35 </t>
         </is>
       </c>
       <c r="C315" t="n">
@@ -4533,7 +4533,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>423,50 €</t>
+          <t xml:space="preserve">423,50 </t>
         </is>
       </c>
       <c r="C316" t="n">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>481,58 €</t>
+          <t xml:space="preserve">481,58 </t>
         </is>
       </c>
       <c r="C317" t="n">
@@ -4559,7 +4559,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>637,67 €</t>
+          <t xml:space="preserve">637,67 </t>
         </is>
       </c>
       <c r="C318" t="n">
@@ -4572,7 +4572,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>393,25 €</t>
+          <t xml:space="preserve">393,25 </t>
         </is>
       </c>
       <c r="C319" t="n">
@@ -4585,7 +4585,7 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>678,81 €</t>
+          <t xml:space="preserve">678,81 </t>
         </is>
       </c>
       <c r="C320" t="n">
@@ -4598,7 +4598,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>417,45 €</t>
+          <t xml:space="preserve">417,45 </t>
         </is>
       </c>
       <c r="C321" t="n">
@@ -4611,7 +4611,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>352,11 €</t>
+          <t xml:space="preserve">352,11 </t>
         </is>
       </c>
       <c r="C322" t="n">
@@ -4624,7 +4624,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>602,58 €</t>
+          <t xml:space="preserve">602,58 </t>
         </is>
       </c>
       <c r="C323" t="n">
@@ -4637,7 +4637,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>1.380,61 €</t>
+          <t xml:space="preserve">1.380,61 </t>
         </is>
       </c>
       <c r="C324" t="n">
@@ -4650,7 +4650,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>983,73 €</t>
+          <t xml:space="preserve">983,73 </t>
         </is>
       </c>
       <c r="C325" t="n">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>759,88 €</t>
+          <t xml:space="preserve">759,88 </t>
         </is>
       </c>
       <c r="C326" t="n">
@@ -4676,7 +4676,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>304,92 €</t>
+          <t xml:space="preserve">304,92 </t>
         </is>
       </c>
       <c r="C327" t="n">
@@ -4689,7 +4689,7 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>648,56 €</t>
+          <t xml:space="preserve">648,56 </t>
         </is>
       </c>
       <c r="C328" t="n">
@@ -4702,7 +4702,7 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>540,87 €</t>
+          <t xml:space="preserve">540,87 </t>
         </is>
       </c>
       <c r="C329" t="n">
@@ -4715,7 +4715,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>286,77 €</t>
+          <t xml:space="preserve">286,77 </t>
         </is>
       </c>
       <c r="C330" t="n">
@@ -4728,7 +4728,7 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>562,65 €</t>
+          <t xml:space="preserve">562,65 </t>
         </is>
       </c>
       <c r="C331" t="n">
@@ -4741,7 +4741,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>544,50 €</t>
+          <t xml:space="preserve">544,50 </t>
         </is>
       </c>
       <c r="C332" t="n">
@@ -4754,7 +4754,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>308,55 €</t>
+          <t xml:space="preserve">308,55 </t>
         </is>
       </c>
       <c r="C333" t="n">
@@ -4767,7 +4767,7 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>376,31 €</t>
+          <t xml:space="preserve">376,31 </t>
         </is>
       </c>
       <c r="C334" t="n">
@@ -4780,7 +4780,7 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>567,49 €</t>
+          <t xml:space="preserve">567,49 </t>
         </is>
       </c>
       <c r="C335" t="n">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>496,10 €</t>
+          <t xml:space="preserve">496,10 </t>
         </is>
       </c>
       <c r="C336" t="n">
@@ -4806,7 +4806,7 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>529,98 €</t>
+          <t xml:space="preserve">529,98 </t>
         </is>
       </c>
       <c r="C337" t="n">
@@ -4819,7 +4819,7 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>401,72 €</t>
+          <t xml:space="preserve">401,72 </t>
         </is>
       </c>
       <c r="C338" t="n">
@@ -4832,7 +4832,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>347,27 €</t>
+          <t xml:space="preserve">347,27 </t>
         </is>
       </c>
       <c r="C339" t="n">
@@ -4845,7 +4845,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>447,70 €</t>
+          <t xml:space="preserve">447,70 </t>
         </is>
       </c>
       <c r="C340" t="n">
@@ -4858,7 +4858,7 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>606,21 €</t>
+          <t xml:space="preserve">606,21 </t>
         </is>
       </c>
       <c r="C341" t="n">
@@ -4871,7 +4871,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>479,16 €</t>
+          <t xml:space="preserve">479,16 </t>
         </is>
       </c>
       <c r="C342" t="n">
@@ -4884,7 +4884,7 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>392,04 €</t>
+          <t xml:space="preserve">392,04 </t>
         </is>
       </c>
       <c r="C343" t="n">
@@ -4897,7 +4897,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>439,23 €</t>
+          <t xml:space="preserve">439,23 </t>
         </is>
       </c>
       <c r="C344" t="n">
@@ -4910,7 +4910,7 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>358,16 €</t>
+          <t xml:space="preserve">358,16 </t>
         </is>
       </c>
       <c r="C345" t="n">
@@ -4923,7 +4923,7 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>348,48 €</t>
+          <t xml:space="preserve">348,48 </t>
         </is>
       </c>
       <c r="C346" t="n">
@@ -4936,7 +4936,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>788,92 €</t>
+          <t xml:space="preserve">788,92 </t>
         </is>
       </c>
       <c r="C347" t="n">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>1.049,07 €</t>
+          <t xml:space="preserve">1.049,07 </t>
         </is>
       </c>
       <c r="C348" t="n">
@@ -4962,7 +4962,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>1.102,31 €</t>
+          <t xml:space="preserve">1.102,31 </t>
         </is>
       </c>
       <c r="C349" t="n">
@@ -4975,7 +4975,7 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>1.386,66 €</t>
+          <t xml:space="preserve">1.386,66 </t>
         </is>
       </c>
       <c r="C350" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>1.118,04 €</t>
+          <t xml:space="preserve">1.118,04 </t>
         </is>
       </c>
       <c r="C351" t="n">
@@ -5001,7 +5001,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>1.393,92 €</t>
+          <t xml:space="preserve">1.393,92 </t>
         </is>
       </c>
       <c r="C352" t="n">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>526,35 €</t>
+          <t xml:space="preserve">526,35 </t>
         </is>
       </c>
       <c r="C353" t="n">
@@ -5027,7 +5027,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>590,48 €</t>
+          <t xml:space="preserve">590,48 </t>
         </is>
       </c>
       <c r="C354" t="n">
@@ -5040,7 +5040,7 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>683,65 €</t>
+          <t xml:space="preserve">683,65 </t>
         </is>
       </c>
       <c r="C355" t="n">
@@ -5053,7 +5053,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>217,80 €</t>
+          <t xml:space="preserve">217,80 </t>
         </is>
       </c>
       <c r="C356" t="n">
@@ -5066,7 +5066,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>257,73 €</t>
+          <t xml:space="preserve">257,73 </t>
         </is>
       </c>
       <c r="C357" t="n">
@@ -5079,7 +5079,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>359,37 €</t>
+          <t xml:space="preserve">359,37 </t>
         </is>
       </c>
       <c r="C358" t="n">
@@ -5092,7 +5092,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>407,77 €</t>
+          <t xml:space="preserve">407,77 </t>
         </is>
       </c>
       <c r="C359" t="n">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>177,87 €</t>
+          <t xml:space="preserve">177,87 </t>
         </is>
       </c>
       <c r="C360" t="n">
@@ -5118,7 +5118,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>284,35 €</t>
+          <t xml:space="preserve">284,35 </t>
         </is>
       </c>
       <c r="C361" t="n">
@@ -5131,7 +5131,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>480,37 €</t>
+          <t xml:space="preserve">480,37 </t>
         </is>
       </c>
       <c r="C362" t="n">
@@ -5144,7 +5144,7 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>580,80 €</t>
+          <t xml:space="preserve">580,80 </t>
         </is>
       </c>
       <c r="C363" t="n">
@@ -5157,7 +5157,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>383,57 €</t>
+          <t xml:space="preserve">383,57 </t>
         </is>
       </c>
       <c r="C364" t="n">
@@ -5170,7 +5170,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>496,10 €</t>
+          <t xml:space="preserve">496,10 </t>
         </is>
       </c>
       <c r="C365" t="n">
@@ -5183,7 +5183,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>330,33 €</t>
+          <t xml:space="preserve">330,33 </t>
         </is>
       </c>
       <c r="C366" t="n">
@@ -5196,7 +5196,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>248,05 €</t>
+          <t xml:space="preserve">248,05 </t>
         </is>
       </c>
       <c r="C367" t="n">
@@ -5209,7 +5209,7 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>435,60 €</t>
+          <t xml:space="preserve">435,60 </t>
         </is>
       </c>
       <c r="C368" t="n">
@@ -5222,7 +5222,7 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>1.593,57 €</t>
+          <t xml:space="preserve">1.593,57 </t>
         </is>
       </c>
       <c r="C369" t="n">
@@ -5235,7 +5235,7 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>1.237,83 €</t>
+          <t xml:space="preserve">1.237,83 </t>
         </is>
       </c>
       <c r="C370" t="n">
@@ -5248,7 +5248,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>2.075,15 €</t>
+          <t xml:space="preserve">2.075,15 </t>
         </is>
       </c>
       <c r="C371" t="n">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>1.362,46 €</t>
+          <t xml:space="preserve">1.362,46 </t>
         </is>
       </c>
       <c r="C372" t="n">
@@ -5274,7 +5274,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>1.497,98 €</t>
+          <t xml:space="preserve">1.497,98 </t>
         </is>
       </c>
       <c r="C373" t="n">
@@ -5287,7 +5287,7 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>1.104,73 €</t>
+          <t xml:space="preserve">1.104,73 </t>
         </is>
       </c>
       <c r="C374" t="n">
@@ -5300,7 +5300,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>1.281,39 €</t>
+          <t xml:space="preserve">1.281,39 </t>
         </is>
       </c>
       <c r="C375" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>1.593,57 €</t>
+          <t xml:space="preserve">1.593,57 </t>
         </is>
       </c>
       <c r="C376" t="n">
@@ -5326,7 +5326,7 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>793,76 €</t>
+          <t xml:space="preserve">793,76 </t>
         </is>
       </c>
       <c r="C377" t="n">
@@ -5339,7 +5339,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>1.132,56 €</t>
+          <t xml:space="preserve">1.132,56 </t>
         </is>
       </c>
       <c r="C378" t="n">
@@ -5352,7 +5352,7 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>1.452,00 €</t>
+          <t xml:space="preserve">1.452,00 </t>
         </is>
       </c>
       <c r="C379" t="n">
@@ -5365,7 +5365,7 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>1.334,63 €</t>
+          <t xml:space="preserve">1.334,63 </t>
         </is>
       </c>
       <c r="C380" t="n">
@@ -5378,7 +5378,7 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>964,37 €</t>
+          <t xml:space="preserve">964,37 </t>
         </is>
       </c>
       <c r="C381" t="n">
@@ -5391,7 +5391,7 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>701,80 €</t>
+          <t xml:space="preserve">701,80 </t>
         </is>
       </c>
       <c r="C382" t="n">
@@ -5404,7 +5404,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>2.008,60 €</t>
+          <t xml:space="preserve">2.008,60 </t>
         </is>
       </c>
       <c r="C383" t="n">
@@ -5417,7 +5417,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>968,00 €</t>
+          <t xml:space="preserve">968,00 </t>
         </is>
       </c>
       <c r="C384" t="n">
@@ -5430,7 +5430,7 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>799,81 €</t>
+          <t xml:space="preserve">799,81 </t>
         </is>
       </c>
       <c r="C385" t="n">
@@ -5443,7 +5443,7 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>1.059,96 €</t>
+          <t xml:space="preserve">1.059,96 </t>
         </is>
       </c>
       <c r="C386" t="n">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>1.059,96 €</t>
+          <t xml:space="preserve">1.059,96 </t>
         </is>
       </c>
       <c r="C387" t="n">
@@ -5469,7 +5469,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>600,16 €</t>
+          <t xml:space="preserve">600,16 </t>
         </is>
       </c>
       <c r="C388" t="n">
@@ -5482,7 +5482,7 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>836,11 €</t>
+          <t xml:space="preserve">836,11 </t>
         </is>
       </c>
       <c r="C389" t="n">
@@ -5495,7 +5495,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>600,16 €</t>
+          <t xml:space="preserve">600,16 </t>
         </is>
       </c>
       <c r="C390" t="n">
@@ -5508,7 +5508,7 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>726,00 €</t>
+          <t xml:space="preserve">726,00 </t>
         </is>
       </c>
       <c r="C391" t="n">
@@ -5521,7 +5521,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>756,25 €</t>
+          <t xml:space="preserve">756,25 </t>
         </is>
       </c>
       <c r="C392" t="n">
@@ -5534,7 +5534,7 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>807,07 €</t>
+          <t xml:space="preserve">807,07 </t>
         </is>
       </c>
       <c r="C393" t="n">
@@ -5547,7 +5547,7 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>876,04 €</t>
+          <t xml:space="preserve">876,04 </t>
         </is>
       </c>
       <c r="C394" t="n">
@@ -5560,7 +5560,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>934,12 €</t>
+          <t xml:space="preserve">934,12 </t>
         </is>
       </c>
       <c r="C395" t="n">
@@ -5573,7 +5573,7 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>193,60 €</t>
+          <t xml:space="preserve">193,60 </t>
         </is>
       </c>
       <c r="C396" t="n">
@@ -5586,7 +5586,7 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>214,17 €</t>
+          <t xml:space="preserve">214,17 </t>
         </is>
       </c>
       <c r="C397" t="n">
@@ -5599,7 +5599,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>385,99 €</t>
+          <t xml:space="preserve">385,99 </t>
         </is>
       </c>
       <c r="C398" t="n">
@@ -5612,7 +5612,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>438,02 €</t>
+          <t xml:space="preserve">438,02 </t>
         </is>
       </c>
       <c r="C399" t="n">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>371,47 €</t>
+          <t xml:space="preserve">371,47 </t>
         </is>
       </c>
       <c r="C400" t="n">
@@ -5638,7 +5638,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>698,17 €</t>
+          <t xml:space="preserve">698,17 </t>
         </is>
       </c>
       <c r="C401" t="n">
@@ -5651,7 +5651,7 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>371,47 €</t>
+          <t xml:space="preserve">371,47 </t>
         </is>
       </c>
       <c r="C402" t="n">
@@ -5664,7 +5664,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>600,16 €</t>
+          <t xml:space="preserve">600,16 </t>
         </is>
       </c>
       <c r="C403" t="n">
@@ -5677,7 +5677,7 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>682,44 €</t>
+          <t xml:space="preserve">682,44 </t>
         </is>
       </c>
       <c r="C404" t="n">
@@ -5690,7 +5690,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>540,87 €</t>
+          <t xml:space="preserve">540,87 </t>
         </is>
       </c>
       <c r="C405" t="n">
@@ -5703,7 +5703,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>912,34 €</t>
+          <t xml:space="preserve">912,34 </t>
         </is>
       </c>
       <c r="C406" t="n">
@@ -5716,7 +5716,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>385,99 €</t>
+          <t xml:space="preserve">385,99 </t>
         </is>
       </c>
       <c r="C407" t="n">
@@ -5729,7 +5729,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>533,61 €</t>
+          <t xml:space="preserve">533,61 </t>
         </is>
       </c>
       <c r="C408" t="n">
@@ -5742,7 +5742,7 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>533,61 €</t>
+          <t xml:space="preserve">533,61 </t>
         </is>
       </c>
       <c r="C409" t="n">
@@ -5755,7 +5755,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>289,19 €</t>
+          <t xml:space="preserve">289,19 </t>
         </is>
       </c>
       <c r="C410" t="n">
@@ -5768,7 +5768,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>429,55 €</t>
+          <t xml:space="preserve">429,55 </t>
         </is>
       </c>
       <c r="C411" t="n">
@@ -5781,7 +5781,7 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>355,74 €</t>
+          <t xml:space="preserve">355,74 </t>
         </is>
       </c>
       <c r="C412" t="n">
@@ -5794,7 +5794,7 @@
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>392,04 €</t>
+          <t xml:space="preserve">392,04 </t>
         </is>
       </c>
       <c r="C413" t="n">
@@ -5807,7 +5807,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>459,80 €</t>
+          <t xml:space="preserve">459,80 </t>
         </is>
       </c>
       <c r="C414" t="n">
@@ -5820,7 +5820,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>526,35 €</t>
+          <t xml:space="preserve">526,35 </t>
         </is>
       </c>
       <c r="C415" t="n">
@@ -5833,7 +5833,7 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>592,90 €</t>
+          <t xml:space="preserve">592,90 </t>
         </is>
       </c>
       <c r="C416" t="n">
@@ -5846,7 +5846,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>526,35 €</t>
+          <t xml:space="preserve">526,35 </t>
         </is>
       </c>
       <c r="C417" t="n">
@@ -5859,7 +5859,7 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>459,80 €</t>
+          <t xml:space="preserve">459,80 </t>
         </is>
       </c>
       <c r="C418" t="n">
@@ -5872,7 +5872,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>444,07 €</t>
+          <t xml:space="preserve">444,07 </t>
         </is>
       </c>
       <c r="C419" t="n">
@@ -5885,7 +5885,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>556,60 €</t>
+          <t xml:space="preserve">556,60 </t>
         </is>
       </c>
       <c r="C420" t="n">
@@ -5898,7 +5898,7 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>698,17 €</t>
+          <t xml:space="preserve">698,17 </t>
         </is>
       </c>
       <c r="C421" t="n">
@@ -5911,7 +5911,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>718,74 €</t>
+          <t xml:space="preserve">718,74 </t>
         </is>
       </c>
       <c r="C422" t="n">
@@ -5924,7 +5924,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>569,91 €</t>
+          <t xml:space="preserve">569,91 </t>
         </is>
       </c>
       <c r="C423" t="n">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>799,81 €</t>
+          <t xml:space="preserve">799,81 </t>
         </is>
       </c>
       <c r="C424" t="n">
@@ -5950,7 +5950,7 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>756,25 €</t>
+          <t xml:space="preserve">756,25 </t>
         </is>
       </c>
       <c r="C425" t="n">
@@ -5963,7 +5963,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>778,03 €</t>
+          <t xml:space="preserve">778,03 </t>
         </is>
       </c>
       <c r="C426" t="n">
@@ -5976,7 +5976,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>799,81 €</t>
+          <t xml:space="preserve">799,81 </t>
         </is>
       </c>
       <c r="C427" t="n">

</xml_diff>